<commit_message>
Made the changes to rectify the error
</commit_message>
<xml_diff>
--- a/TestData/Follo_WebApp_Datas.xlsx
+++ b/TestData/Follo_WebApp_Datas.xlsx
@@ -118,7 +118,7 @@
     <t>Email</t>
   </si>
   <si>
-    <t>followebfullrun005@yopmail.com</t>
+    <t>followebfullrun007@yopmail.com</t>
   </si>
   <si>
     <t>Phone Code</t>
@@ -130,7 +130,7 @@
     <t>Mobile Number</t>
   </si>
   <si>
-    <t>9848546915</t>
+    <t>9848546917</t>
   </si>
   <si>
     <t>First Name</t>
@@ -285,10 +285,10 @@
     <t>Select Project</t>
   </si>
   <si>
-    <t>followebfullrun003@yopmail.com</t>
-  </si>
-  <si>
-    <t>6r#qi35a4@</t>
+    <t>followebfullrun005@yopmail.com</t>
+  </si>
+  <si>
+    <t>6d265@zux!</t>
   </si>
   <si>
     <t>sprintcomplet</t>
@@ -1031,10 +1031,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1128,8 +1128,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1143,14 +1173,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -1160,36 +1182,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1205,7 +1205,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1222,14 +1230,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1283,13 +1283,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1307,25 +1313,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1337,31 +1325,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1373,61 +1379,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1445,7 +1397,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1457,7 +1439,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1512,11 +1512,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1531,21 +1537,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1566,15 +1557,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1586,6 +1568,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1612,7 +1612,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1633,127 +1633,127 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1801,7 +1801,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1874,6 +1873,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2242,7 +2242,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
@@ -2274,7 +2274,7 @@
       <c r="A3" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2282,7 +2282,7 @@
       <c r="A4" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2290,7 +2290,7 @@
       <c r="A5" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2492,7 +2492,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B15" r:id="rId1" display="https://www.edureka.co/community/1579/verifying-whether-element-present-visible-selenium-webdriver"/>
-    <hyperlink ref="B1" r:id="rId2" display="followebfullrun005@yopmail.com" tooltip="mailto:followebfullrun005@yopmail.com"/>
+    <hyperlink ref="B1" r:id="rId2" display="followebfullrun007@yopmail.com" tooltip="mailto:followebfullrun007@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2514,12 +2514,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2574,12 +2574,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2606,21 +2606,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>80</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -2628,10 +2628,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>87</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -2639,10 +2639,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>80</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -2675,12 +2675,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2711,30 +2711,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="32">
         <v>3</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="32">
         <v>2</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2" s="32">
         <v>4</v>
       </c>
     </row>
@@ -2761,19 +2761,19 @@
   </cols>
   <sheetData>
     <row r="1" ht="29" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2781,22 +2781,22 @@
       <c r="A2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="31" t="s">
         <v>112</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="followebfullrun003@yopmail.com" tooltip="mailto:followebfullrun003@yopmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="followebfullrun005@yopmail.com" tooltip="mailto:followebfullrun005@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2818,12 +2818,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2851,7 +2851,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2896,10 +2896,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2936,7 +2936,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2965,24 +2965,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="28.6181818181818" style="42" customWidth="1"/>
-    <col min="2" max="2" width="18.0181818181818" style="42" customWidth="1"/>
+    <col min="1" max="1" width="28.6181818181818" style="41" customWidth="1"/>
+    <col min="2" max="2" width="18.0181818181818" style="41" customWidth="1"/>
     <col min="3" max="3" width="15.0181818181818" customWidth="1"/>
     <col min="4" max="4" width="16.1272727272727" customWidth="1"/>
     <col min="5" max="5" width="30.3454545454545" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -2993,7 +2993,7 @@
       <c r="A2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="43" t="s">
         <v>57</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -3009,7 +3009,7 @@
     <row r="5" spans="2:2">
       <c r="B5" s="44"/>
     </row>
-    <row r="6" spans="3:3">
+    <row r="6" ht="43.5" spans="3:3">
       <c r="C6" s="6" t="s">
         <v>60</v>
       </c>
@@ -3042,11 +3042,11 @@
     <hyperlink ref="C10" r:id="rId3" display="v@8w4h7@l1"/>
     <hyperlink ref="E8" r:id="rId4" display="5p2##69cjf" tooltip="mailto:v@8w4h7@l13"/>
     <hyperlink ref="E7" r:id="rId5" display="sprint7cc001@yopmail.com" tooltip="mailto:sprint7cc001@yopmail.com"/>
-    <hyperlink ref="A2" r:id="rId6" display="followebfullrun003@yopmail.com" tooltip="mailto:followebfullrun003@yopmail.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="6r#qi35a4@"/>
+    <hyperlink ref="A2" r:id="rId6" display="followebfullrun005@yopmail.com" tooltip="mailto:followebfullrun005@yopmail.com"/>
     <hyperlink ref="C2" r:id="rId1" display="sprintcomplet" tooltip="mailto:sprintcomplete004@yopmail.com"/>
     <hyperlink ref="D2" r:id="rId2" display="VGVGVHVHV"/>
     <hyperlink ref="E2" r:id="rId2" display="Automation Testing"/>
+    <hyperlink ref="B2" r:id="rId7" display="6d265@zux!"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3068,7 +3068,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3104,13 +3104,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3121,7 +3121,7 @@
       <c r="B2" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3132,7 +3132,7 @@
       <c r="B3" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3143,7 +3143,7 @@
       <c r="B4" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3176,16 +3176,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3196,10 +3196,10 @@
       <c r="B2" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3227,7 +3227,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3257,7 +3257,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3287,7 +3287,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3408,10 +3408,10 @@
       <c r="H2" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="18" t="s">
         <v>80</v>
       </c>
       <c r="K2" s="11" t="s">
@@ -3464,10 +3464,10 @@
       <c r="H3" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="18" t="s">
         <v>80</v>
       </c>
       <c r="K3" s="11" t="s">
@@ -3520,10 +3520,10 @@
       <c r="H4" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>80</v>
       </c>
       <c r="K4" s="11" t="s">
@@ -3722,10 +3722,10 @@
       <c r="K2" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="18" t="s">
         <v>80</v>
       </c>
       <c r="N2" s="11" t="s">
@@ -3793,7 +3793,7 @@
       <c r="B2" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3814,14 +3814,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.54545454545455" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="19.3636363636364" style="38" customWidth="1"/>
-    <col min="2" max="2" width="19.0909090909091" style="38" customWidth="1"/>
-    <col min="3" max="3" width="11.1818181818182" style="38" customWidth="1"/>
-    <col min="4" max="16370" width="5.54545454545455" style="38" customWidth="1"/>
-    <col min="16371" max="16384" width="5.54545454545455" style="38"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="41" customFormat="1" spans="1:2">
+    <col min="1" max="1" width="19.3636363636364" style="37" customWidth="1"/>
+    <col min="2" max="2" width="19.0909090909091" style="37" customWidth="1"/>
+    <col min="3" max="3" width="11.1818181818182" style="37" customWidth="1"/>
+    <col min="4" max="16370" width="5.54545454545455" style="37" customWidth="1"/>
+    <col min="16371" max="16384" width="5.54545454545455" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="40" customFormat="1" spans="1:2">
       <c r="A1" s="8" t="s">
         <v>65</v>
       </c>
@@ -3830,26 +3830,26 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>72</v>
       </c>
     </row>
@@ -4111,7 +4111,7 @@
       <c r="C2" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4268,12 +4268,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4370,10 +4370,10 @@
       <c r="F2" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="18" t="s">
         <v>80</v>
       </c>
       <c r="I2" s="11" t="s">
@@ -4420,10 +4420,10 @@
       <c r="F3" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>80</v>
       </c>
       <c r="I3" s="11" t="s">
@@ -4579,10 +4579,10 @@
       <c r="G2" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>80</v>
       </c>
       <c r="J2" s="11" t="s">
@@ -4830,7 +4830,7 @@
       <c r="A2" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4872,16 +4872,16 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4949,10 +4949,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>195</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -4985,7 +4985,7 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>197</v>
       </c>
     </row>
@@ -5045,7 +5045,7 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>197</v>
       </c>
     </row>
@@ -5131,10 +5131,10 @@
       </c>
     </row>
     <row r="2" ht="43.5" spans="1:19">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>195</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -5158,10 +5158,10 @@
       <c r="I2" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>202</v>
       </c>
       <c r="L2" s="11" t="s">
@@ -5556,7 +5556,7 @@
       <c r="B2" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -5603,7 +5603,7 @@
       <c r="B3" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>68</v>
       </c>
       <c r="D3" s="13" t="s">
@@ -5660,24 +5660,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="15.8181818181818" style="39" customWidth="1"/>
-    <col min="2" max="2" width="17.5454545454545" style="39" customWidth="1"/>
-    <col min="3" max="16384" width="8.72727272727273" style="39"/>
+    <col min="1" max="1" width="15.8181818181818" style="38" customWidth="1"/>
+    <col min="2" max="2" width="17.5454545454545" style="38" customWidth="1"/>
+    <col min="3" max="16384" width="8.72727272727273" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" s="38" customFormat="1" spans="1:2">
-      <c r="A2" s="40" t="s">
+    <row r="2" s="37" customFormat="1" spans="1:2">
+      <c r="A2" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5756,7 +5756,7 @@
       <c r="B2" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -5933,7 +5933,7 @@
       <c r="E2" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>68</v>
       </c>
       <c r="G2" s="13" t="s">
@@ -6233,7 +6233,7 @@
       <c r="C2" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>186</v>
       </c>
     </row>
@@ -6307,130 +6307,130 @@
   </cols>
   <sheetData>
     <row r="1" ht="29" spans="1:10">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="20" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" ht="29" spans="1:10">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="36" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" ht="29" spans="1:10">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="36" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" ht="29" spans="1:10">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="36" t="s">
         <v>86</v>
       </c>
     </row>
@@ -6510,7 +6510,7 @@
       <c r="B2" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -6557,7 +6557,7 @@
       <c r="B3" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>68</v>
       </c>
       <c r="D3" s="13" t="s">
@@ -6707,7 +6707,7 @@
       <c r="E2" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>68</v>
       </c>
       <c r="G2" s="14" t="s">
@@ -6958,7 +6958,7 @@
       <c r="A2" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>186</v>
       </c>
     </row>
@@ -6983,12 +6983,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>80</v>
       </c>
     </row>
@@ -7082,7 +7082,7 @@
       <c r="D2" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>68</v>
       </c>
       <c r="F2" s="12" t="s">
@@ -7119,25 +7119,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7145,22 +7145,22 @@
       <c r="A2" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>25</v>
       </c>
     </row>
@@ -7187,21 +7187,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>80</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -7241,13 +7241,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>123</v>
       </c>
     </row>
@@ -7258,7 +7258,7 @@
       <c r="B2" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="5" t="s">
         <v>129</v>
       </c>
     </row>
@@ -7302,7 +7302,7 @@
       <c r="A2" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="5" t="s">
         <v>240</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -7750,48 +7750,48 @@
   </cols>
   <sheetData>
     <row r="1" ht="29" spans="1:11">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="33" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" ht="29" spans="1:11">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="14" t="s">
@@ -7806,13 +7806,13 @@
       <c r="G2" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>97</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="34" t="s">
         <v>85</v>
       </c>
       <c r="K2" s="14" t="s">

</xml_diff>